<commit_message>
Filled in the ActivityList.xls chart
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
   <si>
     <t>模块</t>
   </si>
@@ -247,15 +247,9 @@
     <t>陈泽松</t>
   </si>
   <si>
-    <t>UUCampus</t>
-  </si>
-  <si>
     <t>故事脚本</t>
   </si>
   <si>
-    <t>操作手册</t>
-  </si>
-  <si>
     <t>王德宇</t>
   </si>
   <si>
@@ -289,9 +283,6 @@
     <t>领导力人才</t>
   </si>
   <si>
-    <t>郭聪，马老师，徐涛</t>
-  </si>
-  <si>
     <t>何梦新</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
     <t>待定</t>
   </si>
   <si>
-    <t>大数据分析</t>
-  </si>
-  <si>
     <t>王霞</t>
   </si>
   <si>
@@ -401,16 +389,75 @@
   </si>
   <si>
     <t>信息系统人员</t>
+  </si>
+  <si>
+    <t>使用案例</t>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>郭聪，徐涛，马老师（训练中心）</t>
+  </si>
+  <si>
+    <t>马</t>
+  </si>
+  <si>
+    <t>顾学雍，郭聪</t>
+  </si>
+  <si>
+    <t>郭</t>
+  </si>
+  <si>
+    <t>宣</t>
+  </si>
+  <si>
+    <t>付</t>
+  </si>
+  <si>
+    <t>顾</t>
+  </si>
+  <si>
+    <t>大数据趋势分析</t>
+  </si>
+  <si>
+    <t>该公司可以提供git工程师</t>
+  </si>
+  <si>
+    <t>提供故事背景</t>
+  </si>
+  <si>
+    <t>UUCampus 启动程序</t>
+  </si>
+  <si>
+    <t>要写入Git</t>
+  </si>
+  <si>
+    <t>王</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,16 +485,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -455,48 +525,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="33">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="83">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -512,7 +694,32 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -528,6 +735,31 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -857,607 +1089,920 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE45"/>
+  <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="5.1640625" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" customWidth="1"/>
-    <col min="9" max="9" width="5.5" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" customWidth="1"/>
-    <col min="11" max="11" width="3.83203125" customWidth="1"/>
-    <col min="12" max="12" width="4.1640625" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" customWidth="1"/>
-    <col min="14" max="14" width="4.5" customWidth="1"/>
-    <col min="15" max="15" width="5" customWidth="1"/>
-    <col min="16" max="16" width="5.33203125" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" customWidth="1"/>
-    <col min="19" max="19" width="5.83203125" customWidth="1"/>
-    <col min="20" max="20" width="5.33203125" customWidth="1"/>
-    <col min="21" max="21" width="4.83203125" customWidth="1"/>
-    <col min="22" max="22" width="5" customWidth="1"/>
-    <col min="23" max="23" width="4.83203125" customWidth="1"/>
-    <col min="24" max="24" width="5.1640625" customWidth="1"/>
-    <col min="25" max="25" width="4.33203125" customWidth="1"/>
-    <col min="26" max="26" width="4.1640625" customWidth="1"/>
-    <col min="27" max="28" width="3.83203125" customWidth="1"/>
-    <col min="29" max="29" width="3.1640625" customWidth="1"/>
-    <col min="30" max="30" width="4.1640625" customWidth="1"/>
-    <col min="31" max="31" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.1640625" customWidth="1"/>
+    <col min="31" max="31" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:32" ht="17" thickTop="1" thickBot="1">
+      <c r="F1" s="7">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7">
+        <v>3</v>
+      </c>
+      <c r="H1" s="7">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7">
+        <v>5</v>
+      </c>
+      <c r="J1" s="7">
+        <v>6</v>
+      </c>
+      <c r="K1" s="8">
+        <v>7</v>
+      </c>
+      <c r="L1" s="7">
+        <v>1</v>
+      </c>
+      <c r="M1" s="7">
+        <v>2</v>
+      </c>
+      <c r="N1" s="7">
+        <v>3</v>
+      </c>
+      <c r="O1" s="7">
+        <v>4</v>
+      </c>
+      <c r="P1" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>6</v>
+      </c>
+      <c r="R1" s="10">
+        <v>7</v>
+      </c>
+      <c r="S1" s="7">
+        <v>1</v>
+      </c>
+      <c r="T1" s="7">
+        <v>2</v>
+      </c>
+      <c r="U1" s="7">
+        <v>3</v>
+      </c>
+      <c r="V1" s="7">
+        <v>4</v>
+      </c>
+      <c r="W1" s="7">
+        <v>5</v>
+      </c>
+      <c r="X1" s="7">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="10">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA1" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB1" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC1" s="7">
+        <v>4</v>
+      </c>
+      <c r="AD1" s="7">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="7">
+        <v>6</v>
+      </c>
+      <c r="AF1" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F2">
         <v>25</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>26</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>27</v>
       </c>
-      <c r="I1">
+      <c r="I2">
         <v>28</v>
       </c>
-      <c r="J1">
+      <c r="J2">
         <v>29</v>
       </c>
-      <c r="K1">
+      <c r="K2" s="4">
         <v>30</v>
       </c>
-      <c r="L1">
+      <c r="L2">
+        <v>31</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M1">
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="N1">
+      <c r="O2">
         <v>3</v>
       </c>
-      <c r="O1">
+      <c r="P2">
         <v>4</v>
       </c>
-      <c r="P1">
+      <c r="Q2">
         <v>5</v>
       </c>
-      <c r="Q1">
+      <c r="R2" s="3">
         <v>6</v>
       </c>
-      <c r="R1">
+      <c r="S2">
         <v>7</v>
       </c>
-      <c r="S1">
+      <c r="T2">
         <v>8</v>
       </c>
-      <c r="T1">
+      <c r="U2">
         <v>9</v>
       </c>
-      <c r="U1">
+      <c r="V2">
         <v>10</v>
       </c>
-      <c r="V1">
+      <c r="W2">
         <v>11</v>
       </c>
-      <c r="W1">
+      <c r="X2">
         <v>12</v>
       </c>
-      <c r="X1">
+      <c r="Y2" s="3">
         <v>13</v>
       </c>
-      <c r="Y1">
+      <c r="Z2">
         <v>14</v>
       </c>
-      <c r="Z1">
+      <c r="AA2">
         <v>15</v>
       </c>
-      <c r="AA1">
+      <c r="AB2">
         <v>16</v>
       </c>
-      <c r="AB1">
+      <c r="AC2">
         <v>17</v>
       </c>
-      <c r="AC1">
+      <c r="AD2">
         <v>18</v>
       </c>
-      <c r="AD1">
+      <c r="AE2">
         <v>19</v>
       </c>
-      <c r="AE1">
+      <c r="AF2" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:32">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
-      <c r="A3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
-      <c r="A4" s="1" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:32">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:32">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:32">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
-      <c r="A10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:32">
       <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
+        <v>105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:31">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:32">
       <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
-      <c r="A16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="H21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD21" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:30">
+      <c r="A23" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>43</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R23" s="11"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="G29" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32">
+      <c r="A33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32">
+      <c r="A34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32">
+      <c r="A35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:32">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="1:32">
+      <c r="A37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="1:32">
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32">
+      <c r="A39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32">
+      <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:32">
+      <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+    <row r="42" spans="1:32" s="1" customFormat="1">
+      <c r="A42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="K42" s="14"/>
+      <c r="Q42" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="R42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="AF42" s="15"/>
+    </row>
+    <row r="43" spans="1:32" s="1" customFormat="1">
+      <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="K43" s="14"/>
+      <c r="Q43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="AF43" s="15"/>
+    </row>
+    <row r="44" spans="1:32">
+      <c r="A44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="11"/>
+    </row>
+    <row r="45" spans="1:32">
+      <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>117</v>
+    <row r="46" spans="1:32">
+      <c r="A46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified ActivityList for 12/25 progress
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1700" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="筹备期" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="157">
   <si>
     <t>模块</t>
   </si>
@@ -121,9 +121,6 @@
     <t>基础工业训练中心</t>
   </si>
   <si>
-    <t>TEDxTHU</t>
-  </si>
-  <si>
     <t>Unit3D, Processing, Mathematica</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>厂商配合</t>
   </si>
   <si>
-    <t>丁一涵</t>
-  </si>
-  <si>
     <t>毛勇</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>Creative Commons</t>
   </si>
   <si>
-    <t>刘萍</t>
-  </si>
-  <si>
     <t>美术设计</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
     <t>toyhouse.cc</t>
   </si>
   <si>
-    <t>CoMatrix</t>
-  </si>
-  <si>
     <t>成果展示模板</t>
   </si>
   <si>
@@ -280,15 +268,9 @@
     <t>领导力人才</t>
   </si>
   <si>
-    <t>何梦新</t>
-  </si>
-  <si>
     <t>林明宪</t>
   </si>
   <si>
-    <t>李寅</t>
-  </si>
-  <si>
     <t>待定</t>
   </si>
   <si>
@@ -394,9 +376,6 @@
     <t>马</t>
   </si>
   <si>
-    <t>顾学雍，郭聪</t>
-  </si>
-  <si>
     <t>郭</t>
   </si>
   <si>
@@ -412,16 +391,10 @@
     <t>大数据趋势分析</t>
   </si>
   <si>
-    <t>该公司可以提供git工程师</t>
-  </si>
-  <si>
     <t>提供故事背景</t>
   </si>
   <si>
     <t>UUCampus 启动程序</t>
-  </si>
-  <si>
-    <t>要写入Git</t>
   </si>
   <si>
     <t>王</t>
@@ -448,9 +421,6 @@
     </r>
   </si>
   <si>
-    <t>胡德恩, Francois Grey</t>
-  </si>
-  <si>
     <t>王德宇,毛勇</t>
   </si>
   <si>
@@ -460,10 +430,146 @@
     <t>人员名单</t>
   </si>
   <si>
-    <t>郭聪，徐涛，马晓东（训练中心）</t>
-  </si>
-  <si>
     <t>马老师</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>月2日</t>
+    </r>
+  </si>
+  <si>
+    <t>周四开会</t>
+  </si>
+  <si>
+    <t>50cm^2 雏形</t>
+  </si>
+  <si>
+    <t>忻隆</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>配合</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEDxTHU</t>
+    </r>
+  </si>
+  <si>
+    <t>胡德恩, Francois Grey，徐芦平</t>
+  </si>
+  <si>
+    <t>忻</t>
+  </si>
+  <si>
+    <t>预算已接受</t>
+  </si>
+  <si>
+    <r>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>人参与</t>
+    </r>
+  </si>
+  <si>
+    <t>共3人</t>
+  </si>
+  <si>
+    <t>与宣国芹合作</t>
+  </si>
+  <si>
+    <t>清华学生</t>
+  </si>
+  <si>
+    <t>温和</t>
+  </si>
+  <si>
+    <t>倪正民， 温和</t>
+  </si>
+  <si>
+    <t>温和指导</t>
+  </si>
+  <si>
+    <t>温和，郭聪，徐涛，马晓东（训练中心）</t>
+  </si>
+  <si>
+    <t>温</t>
+  </si>
+  <si>
+    <t>温和，郭聪</t>
+  </si>
+  <si>
+    <t>预计30日能来</t>
+  </si>
+  <si>
+    <t>CoMatrix＋Bootstrap</t>
+  </si>
+  <si>
+    <t>李寅，温和</t>
+  </si>
+  <si>
+    <t>朱吴越</t>
+  </si>
+  <si>
+    <t>朱</t>
+  </si>
+  <si>
+    <t>已PPT呈现</t>
+  </si>
+  <si>
+    <t>要写入Git，Infrastructure Proj</t>
+  </si>
+  <si>
+    <t>温和，美院</t>
+  </si>
+  <si>
+    <t>上午10点</t>
+  </si>
+  <si>
+    <t>维澤1月10日到</t>
+  </si>
+  <si>
+    <t>未定</t>
+  </si>
+  <si>
+    <t>2～3实习生</t>
+  </si>
+  <si>
+    <t>演讲录像</t>
+  </si>
+  <si>
+    <t>金汉</t>
   </si>
 </sst>
 </file>
@@ -604,10 +710,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -707,7 +829,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="99">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -749,6 +871,14 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -790,6 +920,14 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1119,13 +1257,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF47"/>
+  <dimension ref="A1:AF48"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1151,85 +1289,85 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17" thickTop="1" thickBot="1">
       <c r="F1" s="7">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7">
+        <v>7</v>
+      </c>
+      <c r="K1" s="8">
+        <v>1</v>
+      </c>
+      <c r="L1" s="7">
         <v>2</v>
       </c>
-      <c r="G1" s="7">
+      <c r="M1" s="7">
         <v>3</v>
       </c>
-      <c r="H1" s="7">
+      <c r="N1" s="7">
         <v>4</v>
       </c>
-      <c r="I1" s="7">
+      <c r="O1" s="7">
         <v>5</v>
       </c>
-      <c r="J1" s="7">
+      <c r="P1" s="7">
         <v>6</v>
       </c>
-      <c r="K1" s="8">
+      <c r="Q1" s="7">
         <v>7</v>
       </c>
-      <c r="L1" s="7">
+      <c r="R1" s="10">
         <v>1</v>
       </c>
-      <c r="M1" s="7">
+      <c r="S1" s="7">
         <v>2</v>
       </c>
-      <c r="N1" s="7">
+      <c r="T1" s="7">
         <v>3</v>
       </c>
-      <c r="O1" s="7">
+      <c r="U1" s="7">
         <v>4</v>
       </c>
-      <c r="P1" s="7">
+      <c r="V1" s="7">
         <v>5</v>
       </c>
-      <c r="Q1" s="7">
+      <c r="W1" s="7">
         <v>6</v>
       </c>
-      <c r="R1" s="10">
+      <c r="X1" s="7">
         <v>7</v>
       </c>
-      <c r="S1" s="7">
+      <c r="Y1" s="10">
         <v>1</v>
       </c>
-      <c r="T1" s="7">
+      <c r="Z1" s="7">
         <v>2</v>
       </c>
-      <c r="U1" s="7">
+      <c r="AA1" s="7">
         <v>3</v>
       </c>
-      <c r="V1" s="7">
+      <c r="AB1" s="7">
         <v>4</v>
       </c>
-      <c r="W1" s="7">
+      <c r="AC1" s="7">
         <v>5</v>
       </c>
-      <c r="X1" s="7">
+      <c r="AD1" s="7">
         <v>6</v>
       </c>
-      <c r="Y1" s="10">
+      <c r="AE1" s="7">
         <v>7</v>
       </c>
-      <c r="Z1" s="7">
+      <c r="AF1" s="10">
         <v>1</v>
-      </c>
-      <c r="AA1" s="7">
-        <v>2</v>
-      </c>
-      <c r="AB1" s="7">
-        <v>3</v>
-      </c>
-      <c r="AC1" s="7">
-        <v>4</v>
-      </c>
-      <c r="AD1" s="7">
-        <v>5</v>
-      </c>
-      <c r="AE1" s="7">
-        <v>6</v>
-      </c>
-      <c r="AF1" s="10">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -1335,16 +1473,18 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1359,13 +1499,13 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>130</v>
@@ -1386,18 +1526,17 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>121</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1410,10 +1549,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -1421,10 +1560,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:32">
@@ -1432,36 +1574,48 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:32">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:32">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -1471,20 +1625,39 @@
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="1" t="s">
@@ -1494,20 +1667,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="K13"/>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
@@ -1517,20 +1680,9 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:32">
       <c r="A15" s="1" t="s">
@@ -1540,10 +1692,12 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1560,15 +1714,16 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="1" t="s">
@@ -1577,15 +1732,23 @@
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>115</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
@@ -1595,23 +1758,32 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>117</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>131</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1632,13 +1804,13 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1661,58 +1833,67 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>31</v>
+      <c r="C21" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="AD22" s="13" t="s">
-        <v>118</v>
+        <v>37</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="R24" s="11"/>
       <c r="S24" s="2"/>
@@ -1724,348 +1905,368 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
+        <v>37</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD25" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+        <v>66</v>
+      </c>
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>120</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>147</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="G30" s="13" t="s">
-        <v>126</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30"/>
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>120</v>
+        <v>62</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="G31" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="33" spans="1:32">
       <c r="A33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="1:32">
       <c r="A34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>120</v>
+        <v>150</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:32">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>120</v>
+        <v>104</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:32">
       <c r="A36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:32">
       <c r="A37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>107</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
+        <v>106</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="38" spans="1:32">
       <c r="A38" s="1" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="K38"/>
     </row>
     <row r="39" spans="1:32">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="K39"/>
     </row>
     <row r="40" spans="1:32">
       <c r="A40" s="1" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:32">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>114</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="42" spans="1:32">
       <c r="A42" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:32" s="1" customFormat="1">
+        <v>79</v>
+      </c>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:32">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="K43" s="14"/>
-      <c r="Q43" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="R43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="AF43" s="15"/>
+        <v>51</v>
+      </c>
     </row>
     <row r="44" spans="1:32" s="1" customFormat="1">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E44" s="12"/>
       <c r="K44" s="14"/>
-      <c r="Q44" s="2" t="s">
-        <v>120</v>
+      <c r="Q44" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="R44" s="15"/>
       <c r="Y44" s="15"/>
       <c r="AF44" s="15"/>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="11"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="K45" s="14"/>
+      <c r="Q45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="R45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="AF45" s="15"/>
     </row>
     <row r="46" spans="1:32">
       <c r="A46" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="11"/>
     </row>
     <row r="47" spans="1:32">
       <c r="A47" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32">
+      <c r="A48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited the ActivityList, and compressed XLPWorkflow.ppt
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="筹备期" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="163">
   <si>
     <t>模块</t>
   </si>
@@ -142,9 +142,6 @@
     <t>毛勇</t>
   </si>
   <si>
-    <t>杨建新</t>
-  </si>
-  <si>
     <t>袁功平</t>
   </si>
   <si>
@@ -350,9 +347,6 @@
   </si>
   <si>
     <t>高中生调度</t>
-  </si>
-  <si>
-    <t>工业工程系代表</t>
   </si>
   <si>
     <t>严京滨</t>
@@ -579,6 +573,21 @@
   </si>
   <si>
     <t>周5开会</t>
+  </si>
+  <si>
+    <t>协调MakeBlock,AutoDesk</t>
+  </si>
+  <si>
+    <t>杨建新，姜楠</t>
+  </si>
+  <si>
+    <t>杨建新，王姣姣</t>
+  </si>
+  <si>
+    <t>失联</t>
+  </si>
+  <si>
+    <t>已跟AutoDeskSandy 联系</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1282,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1483,17 +1492,20 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>161</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1509,19 +1521,21 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
         <v>117</v>
       </c>
-      <c r="B4" t="s">
-        <v>119</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="13" t="s">
+        <v>110</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1536,16 +1550,16 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1559,10 +1573,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -1570,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:32">
@@ -1584,16 +1598,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1602,13 +1616,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1619,13 +1633,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -1636,10 +1650,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1656,16 +1673,16 @@
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1677,7 +1694,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" s="12"/>
       <c r="K13"/>
@@ -1690,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K14"/>
     </row>
@@ -1702,11 +1719,11 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1727,7 +1744,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1743,20 +1760,20 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I17" s="13"/>
     </row>
@@ -1768,15 +1785,15 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1789,10 +1806,10 @@
         <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1820,7 +1837,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1849,64 +1866,67 @@
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G24" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R24" s="11"/>
       <c r="S24" s="2"/>
@@ -1918,41 +1938,41 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AD25" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1962,30 +1982,30 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H28" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1999,19 +2019,19 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2020,45 +2040,45 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E31" s="12"/>
       <c r="G31" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:32">
       <c r="A33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G33" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2076,101 +2096,104 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:32">
       <c r="A35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:32">
       <c r="A36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:32">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:32">
       <c r="A38" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K38" s="16"/>
     </row>
     <row r="39" spans="1:32">
       <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="K39"/>
     </row>
     <row r="40" spans="1:32">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K40"/>
     </row>
@@ -2179,64 +2202,64 @@
         <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:32">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:32">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:32">
       <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:32" s="1" customFormat="1">
       <c r="A45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E45" s="12"/>
       <c r="K45" s="14"/>
       <c r="Q45" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R45" s="15"/>
       <c r="Y45" s="15"/>
@@ -2244,18 +2267,18 @@
     </row>
     <row r="46" spans="1:32" s="1" customFormat="1">
       <c r="A46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="E46" s="12"/>
       <c r="K46" s="14"/>
       <c r="Q46" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R46" s="15"/>
       <c r="Y46" s="15"/>
@@ -2263,10 +2286,10 @@
     </row>
     <row r="47" spans="1:32">
       <c r="A47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
@@ -2282,21 +2305,21 @@
     </row>
     <row r="48" spans="1:32">
       <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the ActivityList, by changing the responsible persons for a few projects.
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="5580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="筹备期" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="173">
   <si>
     <t>模块</t>
   </si>
@@ -605,9 +605,6 @@
     <t>与王姣姣，胡泉玮合作</t>
   </si>
   <si>
-    <t>胡泉玮， 温和</t>
-  </si>
-  <si>
     <t>胡</t>
   </si>
   <si>
@@ -615,6 +612,12 @@
   </si>
   <si>
     <t>Readme.md说明 与案例</t>
+  </si>
+  <si>
+    <t>软件接口模板</t>
+  </si>
+  <si>
+    <t>王德宇</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1317,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1749,10 +1752,10 @@
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
@@ -1858,16 +1861,16 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>168</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>169</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>

</xml_diff>

<commit_message>
Made changes in ActivityList
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="174">
   <si>
     <t>模块</t>
   </si>
@@ -1317,10 +1317,10 @@
   <dimension ref="A1:AF50"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1540,9 +1540,7 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="13" t="s">
-        <v>122</v>
-      </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>

</xml_diff>

<commit_message>
Added changes for TEEP_Annoucement_Meeting
</commit_message>
<xml_diff>
--- a/课程方案/ActivityList.xlsx
+++ b/课程方案/ActivityList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1760" yWindow="-20" windowWidth="25600" windowHeight="21100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="筹备期" sheetId="1" r:id="rId1"/>
@@ -572,9 +572,6 @@
     <t>赵千川，赵明国</t>
   </si>
   <si>
-    <t>张雄</t>
-  </si>
-  <si>
     <t>源代码模板，助教人力支持</t>
   </si>
   <si>
@@ -621,6 +618,9 @@
   </si>
   <si>
     <t>提供技术支持与器材</t>
+  </si>
+  <si>
+    <t>张雄的博士生，陈享</t>
   </si>
 </sst>
 </file>
@@ -1316,17 +1316,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
@@ -1536,7 +1536,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="2"/>
@@ -1558,10 +1558,10 @@
         <v>155</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>156</v>
@@ -1580,16 +1580,16 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="E5" s="12"/>
       <c r="K5" s="17"/>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="G14" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1777,7 +1777,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>34</v>
@@ -1785,11 +1785,11 @@
       <c r="E15" s="12"/>
       <c r="F15" s="2"/>
       <c r="G15" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K15"/>
       <c r="P15" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q15" s="2"/>
     </row>
@@ -1841,7 +1841,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="13" t="s">
@@ -1860,16 +1860,16 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1988,7 +1988,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>70</v>
@@ -2010,7 +2010,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>142</v>
@@ -2052,7 +2052,7 @@
         <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>36</v>
@@ -2412,7 +2412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>